<commit_message>
all old graphs produced, note lead
</commit_message>
<xml_diff>
--- a/data/210429_MESA totals calibration comparison_for Jeff and Emil.xlsx
+++ b/data/210429_MESA totals calibration comparison_for Jeff and Emil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilhafeez/Google Drive/Career/Columbia/MESA/mesa_metals_calibration/mesa_metals_calibration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0652143-66AF-1742-96C7-FC87B94D8A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D49B216-9EEC-804E-A332-08A65148F765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="702" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25520" windowHeight="17500" tabRatio="702" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Co" sheetId="1" r:id="rId1"/>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1879,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4735,8 +4735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A37" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6162,8 +6162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="E16" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6876,7 +6876,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B51" sqref="B51:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7589,7 +7589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11159,7 +11159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>